<commit_message>
chore: log sheet updated
</commit_message>
<xml_diff>
--- a/otherDocs/BegumAksuYilmaz_Assessment-Hour-Log.xlsx
+++ b/otherDocs/BegumAksuYilmaz_Assessment-Hour-Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web_backend_test_catering_api\otherDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98CBDD6-0919-4842-A4A2-C94F1B10AE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8010B0-CE18-4B43-B81C-54954C027C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7965" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="118">
   <si>
     <r>
       <rPr>
@@ -282,6 +282,132 @@
   </si>
   <si>
     <t>Read.me, location and tag deletion correction, unit tests for these, hour log sheet, postman json, ER diagram, adding TOD0's etc</t>
+  </si>
+  <si>
+    <t>Code cleaning</t>
+  </si>
+  <si>
+    <t>testDb, double authentication check, printf debug in unit test removed</t>
+  </si>
+  <si>
+    <t>Make clear response</t>
+  </si>
+  <si>
+    <t>For clearity, reponse is divided more meaningful way. Begin with FacilityController specific field level error messages added. Releated DTO's are corrected.</t>
+  </si>
+  <si>
+    <t>When creating/inserting to multiple tables rollback/transaction logic is added.</t>
+  </si>
+  <si>
+    <t>DB Transaction Mechanism</t>
+  </si>
+  <si>
+    <t>Tag addition Correction</t>
+  </si>
+  <si>
+    <t>Correction for adding tag to a facility when creating it and test logic.</t>
+  </si>
+  <si>
+    <t>Cursor based pagination correction</t>
+  </si>
+  <si>
+    <t>Remove Second Query</t>
+  </si>
+  <si>
+    <t>When getting facilities cursor-based pagination not works properly, corrected.</t>
+  </si>
+  <si>
+    <t>Second query usage in when getting paginated results is eliminated.</t>
+  </si>
+  <si>
+    <t>Tests for cursor based pagination for facility and bug fixes.</t>
+  </si>
+  <si>
+    <t>Cursor encode/decode</t>
+  </si>
+  <si>
+    <t>Cursor encoding/decoding added with related classes.</t>
+  </si>
+  <si>
+    <t>Models Creation</t>
+  </si>
+  <si>
+    <t>Skeleton for models are added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some bug fixes are made (wrong id usage etc.) and debug related things are removed. </t>
+  </si>
+  <si>
+    <t>Facility Model</t>
+  </si>
+  <si>
+    <t>Facility model added with usages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test and bug fixes and </t>
+  </si>
+  <si>
+    <t>Employee Model/ Employee Pagination Correction</t>
+  </si>
+  <si>
+    <t>Employee model added with usages. Get paginated results are also corrected for employees.</t>
+  </si>
+  <si>
+    <t>Employee related response messages</t>
+  </si>
+  <si>
+    <t>Like in facility, specific messages are also added for employee.</t>
+  </si>
+  <si>
+    <t>Test and bug fixes. Also PHPDoc corrections.</t>
+  </si>
+  <si>
+    <t>Tag Model/ Tag Pagination Correction</t>
+  </si>
+  <si>
+    <t>Tag model added with usages and paginated results logic is corrected.</t>
+  </si>
+  <si>
+    <t>Test and bug fixes and some code cleaning is made.</t>
+  </si>
+  <si>
+    <t>Tag related response messages</t>
+  </si>
+  <si>
+    <t>Like in facility, specific messages are also added for tag</t>
+  </si>
+  <si>
+    <t>Location Model/ Location Pagination Correction</t>
+  </si>
+  <si>
+    <t>Location model added with usages and also paginated results are corrected.</t>
+  </si>
+  <si>
+    <t>Location related response messages</t>
+  </si>
+  <si>
+    <t>Like in facility, specific messages are also added for location.</t>
+  </si>
+  <si>
+    <t>Test and bug fixes. Some code cleaning.</t>
+  </si>
+  <si>
+    <t>Enum added</t>
+  </si>
+  <si>
+    <t>Since specific error messages multiple times, enumaration is added.</t>
+  </si>
+  <si>
+    <t>Unit test fixes</t>
+  </si>
+  <si>
+    <t>Since some functions return types or logic is changed, tests are fixed.</t>
+  </si>
+  <si>
+    <t>Postman Collection</t>
+  </si>
+  <si>
+    <t>Rearrange postman collection, made folder by folder.</t>
   </si>
 </sst>
 </file>
@@ -545,7 +671,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -573,9 +699,6 @@
     </xf>
     <xf numFmtId="1" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -587,7 +710,19 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -599,16 +734,13 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1043,38 +1175,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.765625" style="29" customWidth="1"/>
     <col min="2" max="2" width="10.765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.61328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.69140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55.4609375" style="1" customWidth="1"/>
     <col min="5" max="6" width="23.61328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1101,7 +1233,7 @@
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="23">
         <v>45862</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -1114,10 +1246,10 @@
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="20">
         <v>1</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1128,8 +1260,8 @@
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1140,8 +1272,8 @@
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1152,10 +1284,10 @@
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="20">
         <v>1</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="23">
         <v>45863</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1168,8 +1300,8 @@
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
@@ -1180,10 +1312,10 @@
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="20">
         <v>2</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1194,8 +1326,8 @@
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="8" t="s">
         <v>19</v>
       </c>
@@ -1206,8 +1338,8 @@
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
@@ -1218,8 +1350,8 @@
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1230,10 +1362,10 @@
       <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="20">
         <v>2</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1244,8 +1376,8 @@
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1256,9 +1388,9 @@
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="20" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="9"/>
@@ -1268,8 +1400,8 @@
       <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="8" t="s">
         <v>29</v>
       </c>
@@ -1280,10 +1412,10 @@
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="20">
         <v>1</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="8" t="s">
         <v>31</v>
       </c>
@@ -1296,8 +1428,8 @@
       <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="8" t="s">
         <v>32</v>
       </c>
@@ -1310,8 +1442,8 @@
       <c r="A20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="8" t="s">
         <v>34</v>
       </c>
@@ -1324,10 +1456,10 @@
       <c r="A21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="20">
         <v>2</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="23">
         <v>45866</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -1340,8 +1472,8 @@
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1352,8 +1484,8 @@
       <c r="A23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="8" t="s">
         <v>38</v>
       </c>
@@ -1364,8 +1496,8 @@
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="8" t="s">
         <v>19</v>
       </c>
@@ -1376,8 +1508,8 @@
       <c r="A25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="8" t="s">
         <v>41</v>
       </c>
@@ -1388,8 +1520,8 @@
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
@@ -1400,10 +1532,10 @@
       <c r="A27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="25">
+      <c r="B27" s="20">
         <v>1</v>
       </c>
-      <c r="C27" s="28"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="8" t="s">
         <v>43</v>
       </c>
@@ -1416,8 +1548,8 @@
       <c r="A28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="8" t="s">
         <v>44</v>
       </c>
@@ -1430,10 +1562,10 @@
       <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="20">
         <v>2</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="23">
         <v>45867</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -1446,8 +1578,8 @@
       <c r="A30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="8" t="s">
         <v>47</v>
       </c>
@@ -1458,10 +1590,10 @@
       <c r="A31" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="25">
+      <c r="B31" s="20">
         <v>1</v>
       </c>
-      <c r="C31" s="28"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="8" t="s">
         <v>50</v>
       </c>
@@ -1474,8 +1606,8 @@
       <c r="A32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="8" t="s">
         <v>49</v>
       </c>
@@ -1488,10 +1620,10 @@
       <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="20">
         <v>1</v>
       </c>
-      <c r="C33" s="28"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="8" t="s">
         <v>51</v>
       </c>
@@ -1502,8 +1634,8 @@
       <c r="A34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="8" t="s">
         <v>52</v>
       </c>
@@ -1514,10 +1646,10 @@
       <c r="A35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="25">
+      <c r="B35" s="20">
         <v>1</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="8" t="s">
         <v>54</v>
       </c>
@@ -1528,8 +1660,8 @@
       <c r="A36" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="25"/>
       <c r="D36" s="8" t="s">
         <v>55</v>
       </c>
@@ -1540,10 +1672,10 @@
       <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="25">
+      <c r="B37" s="20">
         <v>2</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="23">
         <v>45868</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -1556,8 +1688,8 @@
       <c r="A38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="28"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="8" t="s">
         <v>60</v>
       </c>
@@ -1568,8 +1700,8 @@
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="28"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="8" t="s">
         <v>61</v>
       </c>
@@ -1580,8 +1712,8 @@
       <c r="A40" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="8" t="s">
         <v>62</v>
       </c>
@@ -1595,7 +1727,7 @@
       <c r="B41" s="7">
         <v>1</v>
       </c>
-      <c r="C41" s="28"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="8" t="s">
         <v>63</v>
       </c>
@@ -1609,7 +1741,7 @@
       <c r="B42" s="7">
         <v>1</v>
       </c>
-      <c r="C42" s="28"/>
+      <c r="C42" s="24"/>
       <c r="D42" s="8" t="s">
         <v>65</v>
       </c>
@@ -1620,10 +1752,10 @@
       <c r="A43" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="20">
         <v>1</v>
       </c>
-      <c r="C43" s="28"/>
+      <c r="C43" s="24"/>
       <c r="D43" s="8" t="s">
         <v>67</v>
       </c>
@@ -1636,8 +1768,8 @@
       <c r="A44" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="8" t="s">
         <v>68</v>
       </c>
@@ -1650,11 +1782,11 @@
       <c r="A45" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="18">
         <v>2</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="20" t="s">
+      <c r="C45" s="25"/>
+      <c r="D45" s="19" t="s">
         <v>69</v>
       </c>
       <c r="E45" s="9" t="s">
@@ -1666,10 +1798,10 @@
       <c r="A46" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="19">
+      <c r="B46" s="18">
         <v>2</v>
       </c>
-      <c r="C46" s="21">
+      <c r="C46" s="23">
         <v>45870</v>
       </c>
       <c r="D46" s="8" t="s">
@@ -1687,65 +1819,405 @@
       <c r="B47" s="7">
         <v>2</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="20" t="s">
+      <c r="C47" s="25"/>
+      <c r="D47" s="19" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12"/>
+    <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="20">
+        <v>1</v>
+      </c>
+      <c r="C48" s="23">
+        <v>45882</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="9"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="21"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="9"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="21"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="9"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="20">
+        <v>1</v>
+      </c>
+      <c r="C52" s="24"/>
+      <c r="D52" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" s="9"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="21"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="9"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="21"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="9"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="22"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55" s="9"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="20">
+        <v>3</v>
+      </c>
+      <c r="C56" s="24"/>
+      <c r="D56" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="21"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E59" s="9"/>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="22"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="20">
+        <v>2</v>
+      </c>
+      <c r="C61" s="23">
+        <v>45883</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="9"/>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="21"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E62" s="9"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E63" s="9"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="22"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" s="9"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="20">
+        <v>1</v>
+      </c>
+      <c r="C65" s="24"/>
+      <c r="D65" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="9"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="21"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E66" s="9"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="21"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" s="9"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="22">
+        <v>2</v>
+      </c>
+      <c r="C68" s="24"/>
+      <c r="D68" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="20">
+        <v>2</v>
+      </c>
+      <c r="C69" s="24"/>
+      <c r="D69" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" s="9"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="21"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" s="21"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="30">
+        <v>1</v>
+      </c>
+      <c r="C72" s="23">
+        <v>45884</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" s="30">
+        <v>1</v>
+      </c>
+      <c r="C73" s="25"/>
+      <c r="D73" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B49" s="14">
-        <f>SUMIF(E4:E47,"&lt;&gt;x",B4:B47)</f>
-        <v>19</v>
-      </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="18"/>
+      <c r="B75" s="13">
+        <f>SUMIF(E4:E73,"&lt;&gt;x",B4:B73)</f>
+        <v>33</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="14"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="14"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="15"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C21:C28"/>
-    <mergeCell ref="B14:B17"/>
+  <mergeCells count="30">
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C48:C60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C71"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B52:B55"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:F2"/>
@@ -1762,6 +2234,11 @@
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="C29:C36"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C21:C28"/>
+    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: enum added for response messages/errors
</commit_message>
<xml_diff>
--- a/otherDocs/BegumAksuYilmaz_Assessment-Hour-Log.xlsx
+++ b/otherDocs/BegumAksuYilmaz_Assessment-Hour-Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web_backend_test_catering_api\otherDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8010B0-CE18-4B43-B81C-54954C027C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744E49A0-DBC5-4EF4-97C2-C54E9893EFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13950" yWindow="-19845" windowWidth="23040" windowHeight="13560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="120">
   <si>
     <r>
       <rPr>
@@ -408,6 +408,12 @@
   </si>
   <si>
     <t>Rearrange postman collection, made folder by folder.</t>
+  </si>
+  <si>
+    <t>Enum for response messages</t>
+  </si>
+  <si>
+    <t>Enumaration is added for also reponse errors and success messages.</t>
   </si>
 </sst>
 </file>
@@ -710,30 +716,6 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -742,6 +724,30 @@
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1175,15 +1181,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.765625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="24.765625" style="21" customWidth="1"/>
     <col min="2" max="2" width="10.765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.61328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="55.4609375" style="1" customWidth="1"/>
@@ -1191,22 +1197,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1233,7 +1239,7 @@
       <c r="B4" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="25">
         <v>45862</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -1246,10 +1252,10 @@
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="23">
         <v>1</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
@@ -1260,8 +1266,8 @@
       <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1272,8 +1278,8 @@
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1284,10 +1290,10 @@
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="23">
         <v>1</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="25">
         <v>45863</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1300,8 +1306,8 @@
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
@@ -1312,10 +1318,10 @@
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="23">
         <v>2</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1326,8 +1332,8 @@
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="8" t="s">
         <v>19</v>
       </c>
@@ -1338,8 +1344,8 @@
       <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
@@ -1350,8 +1356,8 @@
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1362,10 +1368,10 @@
       <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="23">
         <v>2</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1376,8 +1382,8 @@
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1388,8 +1394,8 @@
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="19" t="s">
         <v>28</v>
       </c>
@@ -1400,8 +1406,8 @@
       <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="8" t="s">
         <v>29</v>
       </c>
@@ -1412,10 +1418,10 @@
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="23">
         <v>1</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="8" t="s">
         <v>31</v>
       </c>
@@ -1428,8 +1434,8 @@
       <c r="A19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="8" t="s">
         <v>32</v>
       </c>
@@ -1442,8 +1448,8 @@
       <c r="A20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="25"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="8" t="s">
         <v>34</v>
       </c>
@@ -1456,10 +1462,10 @@
       <c r="A21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="23">
         <v>2</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="25">
         <v>45866</v>
       </c>
       <c r="D21" s="8" t="s">
@@ -1472,8 +1478,8 @@
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1484,8 +1490,8 @@
       <c r="A23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="8" t="s">
         <v>38</v>
       </c>
@@ -1496,8 +1502,8 @@
       <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="8" t="s">
         <v>19</v>
       </c>
@@ -1508,8 +1514,8 @@
       <c r="A25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="8" t="s">
         <v>41</v>
       </c>
@@ -1520,8 +1526,8 @@
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
@@ -1532,10 +1538,10 @@
       <c r="A27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="23">
         <v>1</v>
       </c>
-      <c r="C27" s="24"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="8" t="s">
         <v>43</v>
       </c>
@@ -1548,8 +1554,8 @@
       <c r="A28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="25"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="8" t="s">
         <v>44</v>
       </c>
@@ -1562,10 +1568,10 @@
       <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="20">
+      <c r="B29" s="23">
         <v>2</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="25">
         <v>45867</v>
       </c>
       <c r="D29" s="8" t="s">
@@ -1578,8 +1584,8 @@
       <c r="A30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="24"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="8" t="s">
         <v>47</v>
       </c>
@@ -1590,10 +1596,10 @@
       <c r="A31" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="23">
         <v>1</v>
       </c>
-      <c r="C31" s="24"/>
+      <c r="C31" s="27"/>
       <c r="D31" s="8" t="s">
         <v>50</v>
       </c>
@@ -1606,8 +1612,8 @@
       <c r="A32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="24"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="8" t="s">
         <v>49</v>
       </c>
@@ -1620,10 +1626,10 @@
       <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="23">
         <v>1</v>
       </c>
-      <c r="C33" s="24"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="8" t="s">
         <v>51</v>
       </c>
@@ -1634,8 +1640,8 @@
       <c r="A34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="8" t="s">
         <v>52</v>
       </c>
@@ -1646,10 +1652,10 @@
       <c r="A35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="20">
+      <c r="B35" s="23">
         <v>1</v>
       </c>
-      <c r="C35" s="24"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="8" t="s">
         <v>54</v>
       </c>
@@ -1660,8 +1666,8 @@
       <c r="A36" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="25"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="8" t="s">
         <v>55</v>
       </c>
@@ -1672,10 +1678,10 @@
       <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="20">
+      <c r="B37" s="23">
         <v>2</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C37" s="25">
         <v>45868</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -1688,8 +1694,8 @@
       <c r="A38" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="8" t="s">
         <v>60</v>
       </c>
@@ -1700,8 +1706,8 @@
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="27"/>
       <c r="D39" s="8" t="s">
         <v>61</v>
       </c>
@@ -1712,8 +1718,8 @@
       <c r="A40" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="24"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="8" t="s">
         <v>62</v>
       </c>
@@ -1727,7 +1733,7 @@
       <c r="B41" s="7">
         <v>1</v>
       </c>
-      <c r="C41" s="24"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="8" t="s">
         <v>63</v>
       </c>
@@ -1741,7 +1747,7 @@
       <c r="B42" s="7">
         <v>1</v>
       </c>
-      <c r="C42" s="24"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="8" t="s">
         <v>65</v>
       </c>
@@ -1752,10 +1758,10 @@
       <c r="A43" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="23">
         <v>1</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="8" t="s">
         <v>67</v>
       </c>
@@ -1768,8 +1774,8 @@
       <c r="A44" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="24"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="8" t="s">
         <v>68</v>
       </c>
@@ -1785,7 +1791,7 @@
       <c r="B45" s="18">
         <v>2</v>
       </c>
-      <c r="C45" s="25"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="19" t="s">
         <v>69</v>
       </c>
@@ -1801,7 +1807,7 @@
       <c r="B46" s="18">
         <v>2</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="25">
         <v>45870</v>
       </c>
       <c r="D46" s="8" t="s">
@@ -1819,7 +1825,7 @@
       <c r="B47" s="7">
         <v>2</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="19" t="s">
         <v>75</v>
       </c>
@@ -1830,10 +1836,10 @@
       <c r="A48" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="20">
+      <c r="B48" s="23">
         <v>1</v>
       </c>
-      <c r="C48" s="23">
+      <c r="C48" s="25">
         <v>45882</v>
       </c>
       <c r="D48" s="8" t="s">
@@ -1846,8 +1852,8 @@
       <c r="A49" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="24"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="19" t="s">
         <v>79</v>
       </c>
@@ -1858,8 +1864,8 @@
       <c r="A50" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="24"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="8" t="s">
         <v>62</v>
       </c>
@@ -1870,8 +1876,8 @@
       <c r="A51" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="24"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="27"/>
       <c r="D51" s="19" t="s">
         <v>80</v>
       </c>
@@ -1882,10 +1888,10 @@
       <c r="A52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="20">
+      <c r="B52" s="23">
         <v>1</v>
       </c>
-      <c r="C52" s="24"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="8" t="s">
         <v>83</v>
       </c>
@@ -1896,8 +1902,8 @@
       <c r="A53" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="24"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="27"/>
       <c r="D53" s="19" t="s">
         <v>86</v>
       </c>
@@ -1908,8 +1914,8 @@
       <c r="A54" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="24"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="8" t="s">
         <v>87</v>
       </c>
@@ -1920,8 +1926,8 @@
       <c r="A55" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="24"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="19" t="s">
         <v>88</v>
       </c>
@@ -1932,10 +1938,10 @@
       <c r="A56" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="20">
+      <c r="B56" s="23">
         <v>3</v>
       </c>
-      <c r="C56" s="24"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="8" t="s">
         <v>90</v>
       </c>
@@ -1946,8 +1952,8 @@
       <c r="A57" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="24"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="19" t="s">
         <v>92</v>
       </c>
@@ -1958,8 +1964,8 @@
       <c r="A58" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="24"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="8" t="s">
         <v>93</v>
       </c>
@@ -1970,8 +1976,8 @@
       <c r="A59" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="24"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="19" t="s">
         <v>95</v>
       </c>
@@ -1982,8 +1988,8 @@
       <c r="A60" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="25"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="26"/>
       <c r="D60" s="8" t="s">
         <v>62</v>
       </c>
@@ -1994,10 +2000,10 @@
       <c r="A61" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="20">
+      <c r="B61" s="23">
         <v>2</v>
       </c>
-      <c r="C61" s="23">
+      <c r="C61" s="25">
         <v>45883</v>
       </c>
       <c r="D61" s="8" t="s">
@@ -2010,8 +2016,8 @@
       <c r="A62" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="24"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="19" t="s">
         <v>96</v>
       </c>
@@ -2022,8 +2028,8 @@
       <c r="A63" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="24"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="8" t="s">
         <v>100</v>
       </c>
@@ -2034,8 +2040,8 @@
       <c r="A64" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="24"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="27"/>
       <c r="D64" s="19" t="s">
         <v>101</v>
       </c>
@@ -2046,10 +2052,10 @@
       <c r="A65" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="20">
+      <c r="B65" s="23">
         <v>1</v>
       </c>
-      <c r="C65" s="24"/>
+      <c r="C65" s="27"/>
       <c r="D65" s="8" t="s">
         <v>103</v>
       </c>
@@ -2060,8 +2066,8 @@
       <c r="A66" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B66" s="21"/>
-      <c r="C66" s="24"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="19" t="s">
         <v>106</v>
       </c>
@@ -2072,8 +2078,8 @@
       <c r="A67" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B67" s="21"/>
-      <c r="C67" s="24"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="27"/>
       <c r="D67" s="8" t="s">
         <v>104</v>
       </c>
@@ -2084,10 +2090,10 @@
       <c r="A68" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B68" s="22">
+      <c r="B68" s="28">
         <v>2</v>
       </c>
-      <c r="C68" s="24"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="19" t="s">
         <v>108</v>
       </c>
@@ -2098,10 +2104,10 @@
       <c r="A69" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="20">
+      <c r="B69" s="23">
         <v>2</v>
       </c>
-      <c r="C69" s="24"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="8" t="s">
         <v>110</v>
       </c>
@@ -2112,8 +2118,8 @@
       <c r="A70" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="24"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="19" t="s">
         <v>111</v>
       </c>
@@ -2124,8 +2130,8 @@
       <c r="A71" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="25"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="26"/>
       <c r="D71" s="8" t="s">
         <v>113</v>
       </c>
@@ -2136,10 +2142,10 @@
       <c r="A72" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B72" s="30">
+      <c r="B72" s="22">
         <v>1</v>
       </c>
-      <c r="C72" s="23">
+      <c r="C72" s="25">
         <v>45884</v>
       </c>
       <c r="D72" s="19" t="s">
@@ -2148,44 +2154,50 @@
       <c r="E72" s="9"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:6" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B73" s="30">
+        <v>118</v>
+      </c>
+      <c r="B73" s="22">
         <v>1</v>
       </c>
-      <c r="C73" s="25"/>
-      <c r="D73" s="8" t="s">
-        <v>117</v>
+      <c r="C73" s="27"/>
+      <c r="D73" s="19" t="s">
+        <v>119</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="12"/>
+    <row r="74" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" s="22">
+        <v>1</v>
+      </c>
+      <c r="C74" s="26"/>
+      <c r="D74" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E74" s="9"/>
       <c r="F74" s="5"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="13">
-        <f>SUMIF(E4:E73,"&lt;&gt;x",B4:B73)</f>
-        <v>33</v>
-      </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
       <c r="E75" s="12"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="14"/>
-      <c r="B76" s="12"/>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="13">
+        <f>SUMIF(E4:E74,"&lt;&gt;x",B4:B74)</f>
+        <v>34</v>
+      </c>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
@@ -2200,24 +2212,28 @@
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="15"/>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="17"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="15"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C48:C60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:C71"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C21:C28"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:F2"/>
@@ -2234,11 +2250,15 @@
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="C29:C36"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C21:C28"/>
-    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="C48:C60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C71"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="B52:B55"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>